<commit_message>
Now i can read Input / Expect data and convert them to JSON style. TODO: Output JSON into files.
</commit_message>
<xml_diff>
--- a/meta/objects/TableSampleOption3.xlsx
+++ b/meta/objects/TableSampleOption3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C72A7C-24C7-DB4A-868D-C256A018BD05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC6C57B-A923-5A4E-A470-5C95A742E814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33360" yWindow="22560" windowWidth="25440" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>クラス名</t>
   </si>
@@ -358,10 +358,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>integer</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>テーブルサンプルのオプションデータクラスです。</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -382,19 +378,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>ArrayList&lt;Int&gt;()</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>ArrayList&lt;String&gt;()</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>new Array&lt;string&gt;()</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>new Array&lt;number&gt;()</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1329,6 +1317,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1344,12 +1356,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1358,24 +1364,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1790,8 +1778,8 @@
   </sheetPr>
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B45" sqref="A45:B45"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1856,7 +1844,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1876,7 +1864,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
@@ -1909,18 +1897,18 @@
       <c r="O8" s="34"/>
     </row>
     <row r="9" spans="1:17" s="28" customFormat="1">
-      <c r="A9" s="109" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="110"/>
+      <c r="A9" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="118"/>
       <c r="C9" s="103" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" s="104"/>
       <c r="E9" s="104"/>
       <c r="F9" s="105"/>
       <c r="K9" s="28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L9" s="106"/>
       <c r="M9" s="106"/>
@@ -1969,12 +1957,12 @@
         <v>2</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="114" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="116"/>
+      <c r="C12" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="122"/>
       <c r="H12" s="40"/>
       <c r="I12" s="40"/>
       <c r="J12" s="61"/>
@@ -2128,15 +2116,15 @@
       <c r="O19"/>
     </row>
     <row r="20" spans="1:19" s="28" customFormat="1">
-      <c r="A20" s="107" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="108"/>
+      <c r="A20" s="115" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="116"/>
       <c r="C20" s="60" t="s">
         <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E20"/>
       <c r="F20"/>
@@ -2412,22 +2400,22 @@
       <c r="F33" s="97"/>
     </row>
     <row r="34" spans="1:19" s="28" customFormat="1">
-      <c r="A34" s="112" t="s">
+      <c r="A34" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="112" t="s">
+      <c r="B34" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="113" t="s">
+      <c r="D34" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="113" t="s">
+      <c r="E34" s="114" t="s">
         <v>55</v>
       </c>
-      <c r="F34" s="111"/>
+      <c r="F34" s="119"/>
       <c r="G34" s="70"/>
       <c r="H34" s="70"/>
       <c r="I34" s="70"/>
@@ -2435,12 +2423,12 @@
       <c r="K34" s="70"/>
     </row>
     <row r="35" spans="1:19" s="28" customFormat="1">
-      <c r="A35" s="112"/>
-      <c r="B35" s="112"/>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="111"/>
+      <c r="A35" s="108"/>
+      <c r="B35" s="108"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="114"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="119"/>
       <c r="G35" s="70"/>
       <c r="H35" s="70"/>
       <c r="I35" s="70"/>
@@ -2691,73 +2679,73 @@
       <c r="S49" s="15"/>
     </row>
     <row r="50" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A50" s="112" t="s">
+      <c r="A50" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="112" t="s">
+      <c r="B50" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="117" t="s">
+      <c r="C50" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="117" t="s">
+      <c r="D50" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="118" t="s">
+      <c r="E50" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="F50" s="117" t="s">
+      <c r="F50" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="113" t="s">
+      <c r="G50" s="114" t="s">
         <v>49</v>
       </c>
-      <c r="H50" s="113" t="s">
+      <c r="H50" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="I50" s="113" t="s">
+      <c r="I50" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="J50" s="117" t="s">
+      <c r="J50" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="K50" s="118" t="s">
+      <c r="K50" s="109" t="s">
         <v>45</v>
       </c>
-      <c r="L50" s="118" t="s">
+      <c r="L50" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="M50" s="121" t="s">
+      <c r="M50" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="N50" s="121" t="s">
+      <c r="N50" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="O50" s="117" t="s">
+      <c r="O50" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="P50" s="117"/>
+      <c r="P50" s="107"/>
       <c r="Q50" s="16"/>
       <c r="R50" s="17"/>
       <c r="S50" s="9"/>
     </row>
     <row r="51" spans="1:19">
-      <c r="A51" s="112"/>
-      <c r="B51" s="112"/>
-      <c r="C51" s="117"/>
-      <c r="D51" s="117"/>
-      <c r="E51" s="119"/>
-      <c r="F51" s="117"/>
-      <c r="G51" s="113"/>
-      <c r="H51" s="113"/>
-      <c r="I51" s="113"/>
-      <c r="J51" s="117"/>
-      <c r="K51" s="120"/>
-      <c r="L51" s="120"/>
-      <c r="M51" s="122"/>
-      <c r="N51" s="122"/>
-      <c r="O51" s="117"/>
-      <c r="P51" s="117"/>
+      <c r="A51" s="108"/>
+      <c r="B51" s="108"/>
+      <c r="C51" s="107"/>
+      <c r="D51" s="107"/>
+      <c r="E51" s="110"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="114"/>
+      <c r="H51" s="114"/>
+      <c r="I51" s="114"/>
+      <c r="J51" s="107"/>
+      <c r="K51" s="111"/>
+      <c r="L51" s="111"/>
+      <c r="M51" s="113"/>
+      <c r="N51" s="113"/>
+      <c r="O51" s="107"/>
+      <c r="P51" s="107"/>
       <c r="Q51" s="18"/>
       <c r="R51" s="25"/>
       <c r="S51" s="15"/>
@@ -2767,23 +2755,23 @@
         <v>1</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D52" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E52" s="21"/>
       <c r="F52" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G52" s="72"/>
       <c r="H52" s="72"/>
       <c r="I52" s="72"/>
       <c r="J52" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K52" s="21"/>
       <c r="L52" s="66"/>
@@ -2805,23 +2793,23 @@
         <v>2</v>
       </c>
       <c r="B53" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>62</v>
-      </c>
       <c r="D53" s="21" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="E53" s="69"/>
       <c r="F53" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G53" s="73"/>
       <c r="H53" s="73"/>
       <c r="I53" s="73"/>
       <c r="J53" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K53" s="21"/>
       <c r="L53" s="66"/>
@@ -3005,6 +2993,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C12:F12"/>
     <mergeCell ref="O50:P51"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="B50:B51"/>
@@ -3020,15 +3017,6 @@
     <mergeCell ref="G50:G51"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="7">

</xml_diff>